<commit_message>
Mail-Backend & file-frontend source added
</commit_message>
<xml_diff>
--- a/Mail-Backend/Assets/Student_Attendance.xlsx
+++ b/Mail-Backend/Assets/Student_Attendance.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -41,12 +41,6 @@
   </si>
   <si>
     <t xml:space="preserve">99ashwinvel@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rato</t>
-  </si>
-  <si>
-    <t xml:space="preserve">deepakdata07@gmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">Kabilan D</t>
@@ -182,13 +176,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.82421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.9"/>
@@ -239,23 +233,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" display="deepakshankar52@gmail.com"/>
     <hyperlink ref="C3" r:id="rId2" display="99ashwinvel@gmail.com"/>
-    <hyperlink ref="C4" r:id="rId3" display="deepakdata07@gmail.com"/>
-    <hyperlink ref="C5" r:id="rId4" display="kabiland04@gmail.com"/>
+    <hyperlink ref="C4" r:id="rId3" display="kabiland04@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>